<commit_message>
Updates from Prithvi - 01 June
</commit_message>
<xml_diff>
--- a/assets/Runner.xlsx
+++ b/assets/Runner.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prith\IdeaProjects\AutomationFW3\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\IdeaProjects\AutomationFW3\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7CD70A6-F7A6-4B36-9976-5354857A0210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BBF66EE-B3C0-4A9D-9C6A-6063529530C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" xr2:uid="{A7E7923E-96C6-47EE-BB19-F9F77B40AA5E}"/>
+    <workbookView xWindow="1470" yWindow="1470" windowWidth="16200" windowHeight="9308" xr2:uid="{A7E7923E-96C6-47EE-BB19-F9F77B40AA5E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -42,49 +42,49 @@
     <t>Execution</t>
   </si>
   <si>
-    <t>TC_001</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
-    <t>TC_002</t>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Browser</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>firefox</t>
+  </si>
+  <si>
+    <t>Suite</t>
+  </si>
+  <si>
+    <t>Regression</t>
+  </si>
+  <si>
+    <t>Smoke</t>
+  </si>
+  <si>
+    <t>LoginTest</t>
+  </si>
+  <si>
+    <t>TC_004</t>
+  </si>
+  <si>
+    <t>TC_005</t>
+  </si>
+  <si>
+    <t>TC_013</t>
+  </si>
+  <si>
+    <t>TC_015</t>
+  </si>
+  <si>
+    <t>CartTest</t>
   </si>
   <si>
     <t>N</t>
-  </si>
-  <si>
-    <t>Class</t>
-  </si>
-  <si>
-    <t>Method</t>
-  </si>
-  <si>
-    <t>Class A</t>
-  </si>
-  <si>
-    <t>Class B</t>
-  </si>
-  <si>
-    <t>test01</t>
-  </si>
-  <si>
-    <t>test99</t>
-  </si>
-  <si>
-    <t>Browser</t>
-  </si>
-  <si>
-    <t>chrome</t>
-  </si>
-  <si>
-    <t>firefox</t>
-  </si>
-  <si>
-    <t>Data File</t>
-  </si>
-  <si>
-    <t>Data Sheet</t>
   </si>
 </sst>
 </file>
@@ -437,19 +437,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDF40EB2-C747-4630-B0CA-D29281BA60F3}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.3828125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -457,57 +457,102 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" t="s">
-        <v>16</v>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
         <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>